<commit_message>
imported remaining files to db
</commit_message>
<xml_diff>
--- a/decm-data/Tabular Sources/cline_1972_rg_repositories.xlsx
+++ b/decm-data/Tabular Sources/cline_1972_rg_repositories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19403"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bellamy2\Documents\DIGITISATION\Upload to Box\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mest\Git_Materials\historical-gazetteer\decm-data\Tabular Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A5CB4-57A6-479D-8694-D1B41FD8808A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16845" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RGs Repository Listings" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="227">
   <si>
     <t>census</t>
   </si>
@@ -714,7 +715,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,24 +1037,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F195" sqref="F195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>13</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>17</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>22</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>26</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>27</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>28</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>29</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>32</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>39</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>42</v>
       </c>
@@ -1521,7 +1522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>48</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>50</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>51</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>52</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>55</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>58</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>63</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>64</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>65</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>69</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>70</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>71</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>73</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>76</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>77</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>81</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>83</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>89</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>90</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>91</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>92</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>96</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>97</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>98</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>99</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>100</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>103</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>104</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>106</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>110</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>111</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>112</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>115</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>116</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>117</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>118</v>
       </c>
@@ -2483,7 +2484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>121</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>122</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>125</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>126</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>129</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>131</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>135</v>
       </c>
@@ -2665,7 +2666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>139</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>141</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>145</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>146</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>147</v>
       </c>
@@ -2795,7 +2796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>149</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>150</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>151</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>153</v>
       </c>
@@ -2899,7 +2900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>154</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>155</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>158</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>159</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>160</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>161</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>162</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>163</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>165</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>166</v>
       </c>
@@ -3159,7 +3160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>5</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>6</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>8</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>9</v>
       </c>
@@ -3315,7 +3316,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>10</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>19</v>
       </c>
@@ -3367,7 +3368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>25</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>30</v>
       </c>
@@ -3419,7 +3420,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>34</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>37</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>41</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>43</v>
       </c>
@@ -3523,7 +3524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>47</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>49</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>53</v>
       </c>
@@ -3601,7 +3602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>54</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>56</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>59</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>61</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>66</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>67</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>79</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>80</v>
       </c>
@@ -3809,7 +3810,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>85</v>
       </c>
@@ -3835,7 +3836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>86</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>95</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>101</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>102</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>105</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>108</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>120</v>
       </c>
@@ -4069,7 +4070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>130</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>132</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>140</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>148</v>
       </c>
@@ -4173,7 +4174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>152</v>
       </c>
@@ -4199,7 +4200,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2</v>
       </c>
@@ -4225,7 +4226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>3</v>
       </c>
@@ -4251,7 +4252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>7</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>11</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>18</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>149</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>23</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>24</v>
       </c>
@@ -4407,7 +4408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>31</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>33</v>
       </c>
@@ -4459,7 +4460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>35</v>
       </c>
@@ -4485,7 +4486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>38</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>44</v>
       </c>
@@ -4537,7 +4538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>45</v>
       </c>
@@ -4563,7 +4564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>46</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>57</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>60</v>
       </c>
@@ -4641,7 +4642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>62</v>
       </c>
@@ -4667,7 +4668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>68</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>164</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>72</v>
       </c>
@@ -4745,7 +4746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>74</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>75</v>
       </c>
@@ -4797,7 +4798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>78</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>82</v>
       </c>
@@ -4849,7 +4850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>84</v>
       </c>
@@ -4875,7 +4876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>87</v>
       </c>
@@ -4901,7 +4902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>88</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>93</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>94</v>
       </c>
@@ -4979,7 +4980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>107</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>109</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>119</v>
       </c>
@@ -5057,7 +5058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>124</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>127</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>128</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>133</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>134</v>
       </c>
@@ -5187,7 +5188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>136</v>
       </c>
@@ -5213,7 +5214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>137</v>
       </c>
@@ -5239,7 +5240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>138</v>
       </c>
@@ -5265,7 +5266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>142</v>
       </c>
@@ -5291,7 +5292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>143</v>
       </c>
@@ -5317,7 +5318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>144</v>
       </c>
@@ -5343,7 +5344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>156</v>
       </c>
@@ -5369,7 +5370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>157</v>
       </c>
@@ -5395,7 +5396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>164</v>
       </c>
@@ -5421,7 +5422,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>123</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>201</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>202</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>203</v>
       </c>
@@ -5507,7 +5508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>204</v>
       </c>
@@ -5530,7 +5531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>205</v>
       </c>
@@ -5550,7 +5551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>206</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>207</v>
       </c>
@@ -5590,7 +5591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>208</v>
       </c>
@@ -5610,7 +5611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>209</v>
       </c>
@@ -5630,7 +5631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>210</v>
       </c>
@@ -5650,7 +5651,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>211</v>
       </c>
@@ -5670,7 +5671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>212</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>213</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>214</v>
       </c>
@@ -5730,7 +5731,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>215</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>216</v>
       </c>
@@ -5770,7 +5771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>217</v>
       </c>
@@ -5790,7 +5791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>218</v>
       </c>
@@ -5810,7 +5811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>219</v>
       </c>
@@ -5830,7 +5831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>220</v>
       </c>
@@ -5850,7 +5851,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>221</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>222</v>
       </c>
@@ -5890,7 +5891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>223</v>
       </c>
@@ -5910,7 +5911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>224</v>
       </c>
@@ -5930,7 +5931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>225</v>
       </c>
@@ -5950,25 +5951,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
-      <c r="E195" t="s">
-        <v>11</v>
-      </c>
-      <c r="F195" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="225" spans="3:3">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="3:3">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="3:3">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C227" t="s">
         <v>226</v>
       </c>

</xml_diff>